<commit_message>
Overeenkomstsoort map met afgeleide klassen
</commit_message>
<xml_diff>
--- a/Referentiedata/VERA - Referentiedata - 2022-01-21.xlsx
+++ b/Referentiedata/VERA - Referentiedata - 2022-01-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewout\Documents\GitHub\VERA-Standaard\Referentiedata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E5E927-278A-4E47-A002-7B438C36AD31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952A0CC-AD96-47A2-B135-DE9C4EE80590}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7700" uniqueCount="3984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7700" uniqueCount="3988">
   <si>
     <t>Referentiedatasoort</t>
   </si>
@@ -12084,6 +12084,18 @@
   </si>
   <si>
     <t>Zelf inrichten</t>
+  </si>
+  <si>
+    <t>Huurovereenkomst</t>
+  </si>
+  <si>
+    <t>Koopovereenkomst</t>
+  </si>
+  <si>
+    <t>Onderhoudsovereenkomst</t>
+  </si>
+  <si>
+    <t>Serviceovereenkomst</t>
   </si>
 </sst>
 </file>
@@ -12403,6 +12415,128 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -12655,128 +12789,6 @@
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -12791,50 +12803,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1199" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27388343-0A0E-446E-86B4-9C4356EB993E}" name="Tabel1" displayName="Tabel1" ref="A1:K1199" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:K1199" xr:uid="{8B075628-E833-48DC-8779-68AB54AC5BC1}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{845F9FC6-EA7E-42C8-9954-6B75834B5282}" name="Referentiedatasoort" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{ABFA2115-257A-4C72-8D5D-B12F03C0BC13}" name="Sortering" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{017F8304-EA34-4997-B9C6-0CC4A749EC8E}" name="Code" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{5FCF4A52-1B6E-4C5E-B548-F2A741E01617}" name="Naam" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{FD4E69DA-6DD3-465E-AF63-FCD3EDFBE4FB}" name="Omschrijving" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{05BEC66F-0654-4B89-86AD-3AE11C926794}" name="Begindatum" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{148B0657-6F42-4A7B-BF5B-1CCD8E7306FE}" name="Einddatum" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{93FF9809-D60E-48FC-92A6-2C71C2A1ECAD}" name="Parent" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{5F097D6A-6015-4022-A051-0A291A6603CE}" name="Gebruikt in domein(en)" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{1FF550CC-1923-46B2-93A7-941EFC52C297}" name="Bovenliggende referentiedatasoort" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{1129875F-9E1B-4640-BC67-459D3E0312B3}" name="Onderliggende referentiedatasoort" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{845F9FC6-EA7E-42C8-9954-6B75834B5282}" name="Referentiedatasoort" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{ABFA2115-257A-4C72-8D5D-B12F03C0BC13}" name="Sortering" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{017F8304-EA34-4997-B9C6-0CC4A749EC8E}" name="Code" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5FCF4A52-1B6E-4C5E-B548-F2A741E01617}" name="Naam" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{FD4E69DA-6DD3-465E-AF63-FCD3EDFBE4FB}" name="Omschrijving" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{05BEC66F-0654-4B89-86AD-3AE11C926794}" name="Begindatum" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{148B0657-6F42-4A7B-BF5B-1CCD8E7306FE}" name="Einddatum" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{93FF9809-D60E-48FC-92A6-2C71C2A1ECAD}" name="Parent" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{5F097D6A-6015-4022-A051-0A291A6603CE}" name="Gebruikt in domein(en)" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{1FF550CC-1923-46B2-93A7-941EFC52C297}" name="Bovenliggende referentiedatasoort" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{1129875F-9E1B-4640-BC67-459D3E0312B3}" name="Onderliggende referentiedatasoort" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{134535DB-0C84-49A6-9207-49B6358693D2}" name="Tabel2" displayName="Tabel2" ref="A1:D250" totalsRowShown="0" headerRowDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{134535DB-0C84-49A6-9207-49B6358693D2}" name="Tabel2" displayName="Tabel2" ref="A1:D250" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:D250" xr:uid="{834F35E8-0EDE-4D67-B3B2-FF2BB529C443}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D250">
     <sortCondition ref="B2:B250"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5F115F3D-5EE0-4A0A-AD8E-B21AF029F55E}" name="Code" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{AC1B045B-EFE8-49BB-9BD6-FF0BA3A275FD}" name="Land" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{9CAAE2D0-7064-4D5D-A7D4-BD7405EF612D}" name="Nationaliteit" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{6F1EDA3A-E7CA-49C7-A87A-29A3FCF21DEE}" name="Nationaliteit code" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{5F115F3D-5EE0-4A0A-AD8E-B21AF029F55E}" name="Code" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AC1B045B-EFE8-49BB-9BD6-FF0BA3A275FD}" name="Land" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9CAAE2D0-7064-4D5D-A7D4-BD7405EF612D}" name="Nationaliteit" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{6F1EDA3A-E7CA-49C7-A87A-29A3FCF21DEE}" name="Nationaliteit code" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ECE8A42-9897-49F3-BCD4-98BB545EE19D}" name="Tabel3" displayName="Tabel3" ref="A1:B335" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0ECE8A42-9897-49F3-BCD4-98BB545EE19D}" name="Tabel3" displayName="Tabel3" ref="A1:B335" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B335" xr:uid="{B9B5B5C9-142C-48DD-9C1E-B6F166F3D527}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B335">
     <sortCondition ref="B2:B335"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{83EAD583-072E-4C1E-9746-E3107C976AE3}" name="Brinnummer" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{E1DB5926-63C9-4717-B3C4-7F13B39EB18A}" name="Naam onderwijsinstelling" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{83EAD583-072E-4C1E-9746-E3107C976AE3}" name="Brinnummer" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E1DB5926-63C9-4717-B3C4-7F13B39EB18A}" name="Naam onderwijsinstelling" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13167,8 +13179,8 @@
   <dimension ref="A1:L1199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1171" sqref="A1171"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31882,7 +31894,7 @@
         <v>30</v>
       </c>
       <c r="D812" s="13" t="s">
-        <v>159</v>
+        <v>3984</v>
       </c>
       <c r="E812" s="15" t="s">
         <v>1656</v>
@@ -31932,7 +31944,7 @@
         <v>160</v>
       </c>
       <c r="D814" s="13" t="s">
-        <v>161</v>
+        <v>3985</v>
       </c>
       <c r="E814" s="15" t="s">
         <v>1659</v>
@@ -31982,7 +31994,7 @@
         <v>129</v>
       </c>
       <c r="D816" s="13" t="s">
-        <v>200</v>
+        <v>3986</v>
       </c>
       <c r="E816" s="15" t="s">
         <v>1663</v>
@@ -32007,7 +32019,7 @@
         <v>141</v>
       </c>
       <c r="D817" s="13" t="s">
-        <v>1664</v>
+        <v>3987</v>
       </c>
       <c r="E817" s="15" t="s">
         <v>1665</v>
@@ -46795,18 +46807,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47013,18 +47025,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6EB239C-D482-4083-A20F-2310AB45B47F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E3AA29B-E85A-4662-AF70-E41EEBB4502A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>